<commit_message>
Nombres de Totems y Delegation Board
</commit_message>
<xml_diff>
--- a/Sprint 3/Delecation Board.xlsx
+++ b/Sprint 3/Delecation Board.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.villaverdee\Documents\GitHub\SpaceInvaders2018\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{96A30A5F-2D43-4C05-9041-A29822BE2FA4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A46627-2D5D-4B0E-810C-45E8AC65768A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{E5C9DF9C-6967-4C24-A87C-138A9637041B}"/>
   </bookViews>
@@ -30,16 +30,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>DECISIONES</t>
+  </si>
+  <si>
+    <t>Delegation Board</t>
+  </si>
+  <si>
+    <t>Work Expo</t>
+  </si>
+  <si>
+    <t>Roadmap con Epics</t>
+  </si>
+  <si>
+    <t>Retrospectiva</t>
+  </si>
+  <si>
+    <t>Selfie Ranking</t>
+  </si>
+  <si>
+    <t>Transpase de bordes de la nave</t>
+  </si>
+  <si>
+    <t>Mapa de HU con RealTimeBoard</t>
+  </si>
+  <si>
+    <t>Planing Poker</t>
+  </si>
+  <si>
+    <t>Limite WIP</t>
+  </si>
+  <si>
+    <t>Música</t>
+  </si>
+  <si>
+    <t>Reiniciar</t>
+  </si>
+  <si>
+    <t>Gestión PB con CA Agile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +97,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -70,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -78,14 +129,180 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -257,16 +474,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>10441</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1577984</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1569721</xdr:colOff>
+      <xdr:colOff>1558835</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2170060</xdr:rowOff>
+      <xdr:rowOff>2162440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -295,7 +512,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4788181" y="7620"/>
+          <a:off x="4778384" y="0"/>
           <a:ext cx="1559280" cy="2162440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -308,22 +525,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>15660</xdr:colOff>
+      <xdr:colOff>54429</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1527484</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2178551</xdr:rowOff>
+      <xdr:rowOff>2166257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagen 10">
+        <xdr:cNvPr id="8" name="Imagen 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88C12CEA-184A-4762-9783-C40115074911}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C928693-EDA2-42B9-9010-E028B5B1853D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -332,7 +549,95 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6422572" y="0"/>
+          <a:ext cx="1473055" cy="2166257"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1588104</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2177143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3B2C1B6-9714-4B5F-B55C-BD18C823EC08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8011885" y="0"/>
+          <a:ext cx="1511905" cy="2177143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>97971</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1660739</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2163311</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3ECDB22-774B-435C-BE00-B3F6F6521F82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -345,8 +650,591 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6385980" y="15240"/>
-          <a:ext cx="1561680" cy="2163311"/>
+          <a:off x="9688285" y="0"/>
+          <a:ext cx="1562768" cy="2163311"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2220685</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>979715</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Gráfico 11" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C02CC9B9-E0F7-434D-8E9C-F6C11EF56D2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3744686" y="2220685"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>250372</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>968829</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Gráfico 12" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ADE3799-DD65-478E-B0BB-682851294750}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5312229" y="2525486"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>272142</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>968829</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Gráfico 13" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{650B8581-C84E-45E0-9CCB-AC640B6B9F6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5312229" y="2873828"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>272143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>968829</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Gráfico 14" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A107A2F5-12C3-4004-A03E-7F788D2A87B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5312229" y="3200400"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>65314</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>968829</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>500743</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Gráfico 15" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94F8A0AD-07F1-4C2D-A153-FBF2C672FB3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="533400" y="3973285"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>566057</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1001486</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>533401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Gráfico 16" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A08E452E-EFF6-45F8-A1CF-28A6855982FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2155371" y="4659086"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>576944</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>587828</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1012373</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>29687</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Gráfico 17" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE45FB83-0FF0-4E00-BE11-0ADE6DB67AB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3777344" y="5148942"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>555172</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>272144</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>990601</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>54430</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Gráfico 18" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D22C89-A0E8-4914-B9A4-D3B7403C4FB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5334001" y="5486401"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>566057</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>272142</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1001486</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Gráfico 19" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{859F21D3-B607-4D81-BC32-E9118859BB40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2155371" y="5812971"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>566057</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>272143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1001486</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Gráfico 20" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA01F3F6-AB8F-4634-A03F-161864648350}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2155371" y="6139543"/>
+          <a:ext cx="435429" cy="435429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>554182</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>277092</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>989611</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>53441</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Gráfico 22" descr="Señal de pulgar hacia arriba">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C707F2E8-0780-49FF-8842-9AF6DE24D03B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5334000" y="6511637"/>
+          <a:ext cx="435429" cy="441367"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -655,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF6D0B3-3EF5-4EBB-96CC-D900BA44710D}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,142 +1555,207 @@
     <col min="2" max="2" width="23.44140625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="23.21875" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="8" max="8" width="39.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="178.8" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="1:8" ht="178.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+    <row r="2" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+    <row r="3" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+    <row r="4" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+    <row r="5" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+    <row r="6" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+    <row r="7" spans="1:8" ht="52.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="10" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+    <row r="8" spans="1:8" ht="52.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="10" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+    <row r="9" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+    <row r="10" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+    <row r="11" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+    <row r="12" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+    <row r="13" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+    <row r="14" spans="1:8" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>